<commit_message>
Updated MB genre labeling tool
</commit_message>
<xml_diff>
--- a/data_processed/ExampleData.xlsx
+++ b/data_processed/ExampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tristan\Documents\Stevens Institute\CPE695\Project\AI-genre-prediction\data_processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB36F7-B4D3-41C5-B1E4-9FF53C463139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA73AF82-3C22-4BF6-AA9B-101384627D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6529CB4-8DDE-4FC9-9766-B2D0C1164C9B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{C6529CB4-8DDE-4FC9-9766-B2D0C1164C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Desired Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="272">
   <si>
     <t xml:space="preserve">analysis_sample_rate </t>
   </si>
@@ -798,9 +798,6 @@
     <t>interval2_count</t>
   </si>
   <si>
-    <t>interval0_count</t>
-  </si>
-  <si>
     <t>interval3_count</t>
   </si>
   <si>
@@ -847,6 +844,15 @@
   </si>
   <si>
     <t>3. Parse interval array into columns based on how many times each interval appears</t>
+  </si>
+  <si>
+    <t>Song title</t>
+  </si>
+  <si>
+    <t>Album/Single/EP</t>
+  </si>
+  <si>
+    <t>interval12_count</t>
   </si>
 </sst>
 </file>
@@ -985,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1007,11 +1013,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,54 +1329,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F3483-8C17-4914-8059-43719F69286C}">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="28" width="16.21875" customWidth="1"/>
-    <col min="30" max="30" width="21.109375" customWidth="1"/>
-    <col min="31" max="31" width="20.33203125" customWidth="1"/>
-    <col min="32" max="32" width="44.88671875" customWidth="1"/>
-    <col min="33" max="33" width="27.6640625" customWidth="1"/>
-    <col min="34" max="34" width="16.21875" customWidth="1"/>
-    <col min="35" max="35" width="14.5546875" customWidth="1"/>
-    <col min="36" max="36" width="16.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="28" width="16.28515625" customWidth="1"/>
+    <col min="30" max="30" width="21.140625" customWidth="1"/>
+    <col min="31" max="31" width="20.28515625" customWidth="1"/>
+    <col min="32" max="32" width="44.85546875" customWidth="1"/>
+    <col min="33" max="33" width="27.7109375" customWidth="1"/>
+    <col min="34" max="34" width="16.28515625" customWidth="1"/>
+    <col min="35" max="35" width="14.5703125" customWidth="1"/>
+    <col min="36" max="36" width="16.42578125" customWidth="1"/>
     <col min="37" max="37" width="16" customWidth="1"/>
-    <col min="39" max="39" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.33203125" customWidth="1"/>
-    <col min="45" max="45" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.28515625" customWidth="1"/>
+    <col min="45" max="45" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="22" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="14" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O1" t="s">
         <v>249</v>
       </c>
@@ -1383,10 +1384,10 @@
         <v>250</v>
       </c>
       <c r="R1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>240</v>
       </c>
@@ -1432,14 +1433,14 @@
       <c r="O2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>253</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>252</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>254</v>
@@ -1466,9 +1467,8 @@
         <v>261</v>
       </c>
       <c r="AA2" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="AB2" s="19"/>
+        <v>271</v>
+      </c>
       <c r="AD2" t="s">
         <v>4</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>241</v>
       </c>
@@ -1621,43 +1621,42 @@
       <c r="O3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="W3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="Z3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB3" s="17"/>
+      <c r="P3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="AD3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1764,7 +1763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>243</v>
       </c>
@@ -1810,43 +1809,42 @@
       <c r="O4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="R4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="S4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="V4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="W4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="X4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Z4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="AA4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB4" s="18"/>
+      <c r="P4" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>267</v>
+      </c>
+      <c r="R4" t="s">
+        <v>267</v>
+      </c>
+      <c r="S4" t="s">
+        <v>267</v>
+      </c>
+      <c r="T4" t="s">
+        <v>267</v>
+      </c>
+      <c r="U4" t="s">
+        <v>267</v>
+      </c>
+      <c r="V4" t="s">
+        <v>267</v>
+      </c>
+      <c r="W4" t="s">
+        <v>267</v>
+      </c>
+      <c r="X4" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>267</v>
+      </c>
       <c r="AD4">
         <v>0.63063003758980696</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>248</v>
       </c>
@@ -1999,43 +1997,42 @@
       <c r="O5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="S5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="T5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="U5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="W5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="X5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="Z5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="AA5" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB5" s="18"/>
+      <c r="P5" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>267</v>
+      </c>
+      <c r="R5" t="s">
+        <v>267</v>
+      </c>
+      <c r="S5" t="s">
+        <v>267</v>
+      </c>
+      <c r="T5" t="s">
+        <v>267</v>
+      </c>
+      <c r="U5" t="s">
+        <v>267</v>
+      </c>
+      <c r="V5" t="s">
+        <v>267</v>
+      </c>
+      <c r="W5" t="s">
+        <v>267</v>
+      </c>
+      <c r="X5" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>267</v>
+      </c>
       <c r="AD5">
         <v>0.48735679092814699</v>
       </c>
@@ -2142,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>245</v>
       </c>
@@ -2188,19 +2185,6 @@
       <c r="O6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
       <c r="AD6">
         <v>0.63038233414678002</v>
       </c>
@@ -2307,7 +2291,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>244</v>
       </c>
@@ -2353,21 +2337,9 @@
       <c r="O7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="P7" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
+      <c r="P7" t="s">
+        <v>263</v>
+      </c>
       <c r="AD7">
         <v>0.65104566083179405</v>
       </c>
@@ -2474,7 +2446,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>242</v>
       </c>
@@ -2520,21 +2492,9 @@
       <c r="O8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="P8" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
+      <c r="P8" t="s">
+        <v>264</v>
+      </c>
       <c r="AD8">
         <v>0.535292735511819</v>
       </c>
@@ -2641,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>246</v>
       </c>
@@ -2687,21 +2647,9 @@
       <c r="O9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="P9" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
+      <c r="P9" t="s">
+        <v>265</v>
+      </c>
       <c r="AD9">
         <v>0.55649560191295699</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" t="s">
         <v>187</v>
@@ -2852,21 +2800,9 @@
       <c r="O10" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="P10" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
+      <c r="P10" t="s">
+        <v>266</v>
+      </c>
       <c r="AD10">
         <v>0.80113644699668696</v>
       </c>
@@ -2973,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" t="s">
         <v>201</v>
@@ -3017,21 +2953,9 @@
       <c r="O11" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="P11" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
+      <c r="P11" t="s">
+        <v>268</v>
+      </c>
       <c r="AD11">
         <v>0.42666785706940502</v>
       </c>
@@ -3138,7 +3062,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" t="s">
         <v>214</v>
@@ -3182,19 +3106,6 @@
       <c r="O12" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
       <c r="AD12">
         <v>0.55051369784821302</v>
       </c>
@@ -3301,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>229</v>
@@ -3345,19 +3256,6 @@
       <c r="O13" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
       <c r="AD13">
         <v>0.36003116646435102</v>
       </c>
@@ -3474,64 +3372,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4114ED32-0CD3-46EE-9918-46C768A165F2}">
   <dimension ref="A1:BB27"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:BB12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="44.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="42.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.77734375" customWidth="1"/>
-    <col min="12" max="12" width="27.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="42.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" customWidth="1"/>
-    <col min="20" max="21" width="11.77734375" customWidth="1"/>
-    <col min="22" max="22" width="13.88671875" customWidth="1"/>
-    <col min="23" max="23" width="14.21875" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="20" max="21" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
     <col min="26" max="26" width="6" customWidth="1"/>
-    <col min="27" max="27" width="16.21875" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
     <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="8.109375" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" customWidth="1"/>
     <col min="31" max="31" width="20" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" customWidth="1"/>
-    <col min="33" max="33" width="18.77734375" customWidth="1"/>
-    <col min="34" max="34" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.7109375" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="26" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.77734375" customWidth="1"/>
+    <col min="39" max="39" width="18.7109375" customWidth="1"/>
     <col min="40" max="40" width="16" customWidth="1"/>
-    <col min="41" max="41" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.44140625" customWidth="1"/>
-    <col min="44" max="44" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.33203125" customWidth="1"/>
-    <col min="46" max="46" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.6640625" customWidth="1"/>
-    <col min="50" max="50" width="25.5546875" customWidth="1"/>
-    <col min="51" max="51" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="28.5546875" customWidth="1"/>
+    <col min="41" max="41" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.42578125" customWidth="1"/>
+    <col min="44" max="44" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.28515625" customWidth="1"/>
+    <col min="46" max="46" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.7109375" customWidth="1"/>
+    <col min="50" max="50" width="25.5703125" customWidth="1"/>
+    <col min="51" max="51" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3695,7 +3593,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3859,7 +3757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22050</v>
       </c>
@@ -4023,7 +3921,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22050</v>
       </c>
@@ -4187,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>22050</v>
       </c>
@@ -4351,7 +4249,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>22050</v>
       </c>
@@ -4515,7 +4413,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22050</v>
       </c>
@@ -4679,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22050</v>
       </c>
@@ -4843,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22050</v>
       </c>
@@ -5007,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22050</v>
       </c>
@@ -5171,7 +5069,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22050</v>
       </c>
@@ -5335,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22050</v>
       </c>
@@ -5499,8 +5397,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>240</v>
       </c>
@@ -5547,7 +5452,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>241</v>
       </c>
@@ -5627,7 +5532,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>243</v>
       </c>
@@ -5707,7 +5612,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>248</v>
       </c>
@@ -5751,7 +5656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>245</v>
       </c>
@@ -5795,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>244</v>
       </c>
@@ -5839,7 +5744,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>242</v>
       </c>
@@ -5883,7 +5788,7 @@
         <v>0.45400000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>246</v>
       </c>
@@ -5927,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" t="s">
         <v>187</v>
@@ -5969,7 +5874,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" t="s">
         <v>201</v>
@@ -6011,7 +5916,7 @@
         <v>0.48699999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" t="s">
         <v>214</v>
@@ -6053,7 +5958,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" t="s">
         <v>229</v>

</xml_diff>